<commit_message>
1) Add capability to "remove all geodata" from files. - Added a new button for the above.
2) logic fixes
3) formatting fixes
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09567DA-D11C-49D8-9157-DE0AE098C3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52774D67-3558-4E13-B0F0-5FF2280E9000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" firstSheet="4" activeTab="12" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="180">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -575,6 +575,18 @@
   </si>
   <si>
     <t>Paste All Geodata</t>
+  </si>
+  <si>
+    <t>btn_RemoveGeoData</t>
+  </si>
+  <si>
+    <t>Remove GeoData</t>
+  </si>
+  <si>
+    <t>Edit File</t>
+  </si>
+  <si>
+    <t>btn_EditFile</t>
   </si>
 </sst>
 </file>
@@ -967,11 +979,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D057A75-CE07-4B70-81C2-6848CE46E100}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:C9"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1070,6 +1082,22 @@
       </c>
       <c r="C11" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1243,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9929B90B-AD05-4D51-B814-E736A13F0538}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -1415,7 +1443,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C32"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add "Remove GeoData" to frm_editFileData
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52774D67-3558-4E13-B0F0-5FF2280E9000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADDC43B-1207-44F7-B63F-4F3B863B7CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
@@ -580,13 +580,13 @@
     <t>btn_RemoveGeoData</t>
   </si>
   <si>
-    <t>Remove GeoData</t>
-  </si>
-  <si>
     <t>Edit File</t>
   </si>
   <si>
     <t>btn_EditFile</t>
+  </si>
+  <si>
+    <t>Remove All Location Data</t>
   </si>
 </sst>
 </file>
@@ -983,7 +983,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
@@ -1097,7 +1097,7 @@
         <v>176</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add message box handling to languages
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="g:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADDC43B-1207-44F7-B63F-4F3B863B7CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5DB26-E407-4BF4-B218-8CB611EE990B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" activeTab="6" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="252">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Write</t>
   </si>
   <si>
-    <t>mbx</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -587,6 +584,230 @@
   </si>
   <si>
     <t>Remove All Location Data</t>
+  </si>
+  <si>
+    <t>This needs to have numbers only. Will default to zero.</t>
+  </si>
+  <si>
+    <t>The app encountered errors communicating with the API. If you got an Unauthorised error, pls set your username as password in the settings.</t>
+  </si>
+  <si>
+    <t>Data Updated.</t>
+  </si>
+  <si>
+    <t>Your files seem to have disappeared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error loading webview2 - Have you installed it?: </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeComponent</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorDoubleBuffer</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorLanguageFileColumnHeaders</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorClearingFileDataQTables</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorResizingColumns</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorSettingStartupFolder</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewEnsureCoreWebView2Async</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewIsWebMessageEnabled</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewReadHTMLFile</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewParseCoordsFromHTMLFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will be a bug.  Please file an issue on github and that the 'sender' was: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed to read default values from SQL (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loading data from SQL Failed (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created but can't write SQLite database (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can't create SQLite database (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoubleBuffer Error (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error clearing the filedata-Q tables (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resizing Columns failed (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting Default Startup folder failed (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitializeComponent (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (await wbv_MapArea.EnsureCoreWebView2Async(c2wv)) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (IsWebMessageEnabled) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (reading HTMLCode file) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (parsing coordinates from HTMLCode file) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewReplaceStringInHTMLFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (replacing constants in HTMLCode file) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewNavigateToStringInHTMLFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.InitialiseWebView (NavigateToString in HTMLCode file) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInitializeWebViewWebMessageReceived</t>
+  </si>
+  <si>
+    <t>Some data has been changed - want to save? 
+Data will be discarded if you click No</t>
+  </si>
+  <si>
+    <t>Do you want to also assign Altitude &amp; Toponomy values?
+If you pick No, your lat/long data may become out of sync with any embedded toponomy data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in frm_mainApp.NavigateMapGo (string HTMLCode) (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorNavigateMapGoHTMLCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The folder you entered doesn't seem valid. (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There was an error reading the language file and assigning columnheaders (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorInvalidFolder</t>
+  </si>
+  <si>
+    <t>Your folder and/or file list contains nonstandard characters.
+These will need to be run in 'compatibility mode', which is slower. 
+Suggesting renaming your path and/or files if you have a large number of item.
+Press OK to continue and be reminded again or Cancel to continue and not be reminded again about this.</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_QuestionDontShowIncompatibleFileWarningAgain</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_QuestionAddToponomy</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_QuestionFileQIsNotEmpty</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorCantCreateSQLiteDB</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorCantWriteSQLiteDB</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorCantLoadSQLiteDB</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorCantReadDefaultSQLiteDB</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorCantLoadWebView2</t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_ErrorFileGoneMissing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File no longer appears to exist: </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_WarningNoItemSelected</t>
+  </si>
+  <si>
+    <t>No Item selected.</t>
+  </si>
+  <si>
+    <t>mbx_frm_editFileData_WarningLatLongMustBeNumbers</t>
+  </si>
+  <si>
+    <t>mbx_frm_editFileData_ErrorAPIError</t>
+  </si>
+  <si>
+    <t>mbx_frm_editFileData_ErrorInvalidSender</t>
+  </si>
+  <si>
+    <t>mbx_frm_editFileData_WarningFileDisappeared</t>
+  </si>
+  <si>
+    <t>mbx_frm_editFileData_InfoDataUpdated</t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningNoARCGISKey</t>
+  </si>
+  <si>
+    <t>You'll need to provide an ArcGIS API Key in the Settings for the app to work properly.</t>
+  </si>
+  <si>
+    <t>mbx_Helper_ErrorAsyncExifToolExecuteAsyncFailed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asyncExifTool.ExecuteAsync failed (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_Helper_ErrorCantReadDefaultSQLiteDB</t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningGeoNamesAPIResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoNames API Returned the following response: </t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningFileDisappeared</t>
+  </si>
+  <si>
+    <t>mbx_Helper_QuestionFileQIsNotEmpty</t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningTooManyFilesSelected</t>
+  </si>
+  <si>
+    <t>This will only work if you have one and only one file selected.</t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningNothingToPaste</t>
+  </si>
+  <si>
+    <t>Nothing to Paste.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error while performing  wbv_MapArea_WebMessageReceived (Please file an issue on github): </t>
   </si>
 </sst>
 </file>
@@ -657,13 +878,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,7 +1208,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
@@ -1009,7 +1236,7 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1017,7 +1244,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1025,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1033,71 +1260,71 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
         <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" t="s">
         <v>170</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" t="s">
         <v>158</v>
-      </c>
-      <c r="C10" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" t="s">
         <v>167</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1108,6 +1335,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474FB6B0-1C4C-4EF7-88E9-FF86336714E7}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1135,10 +1363,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1178,7 +1406,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1186,7 +1414,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1194,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1202,15 +1430,15 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1259,7 +1487,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1269,6 +1497,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9929B90B-AD05-4D51-B814-E736A13F0538}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1296,82 +1525,82 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
         <v>148</v>
-      </c>
-      <c r="C2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>163</v>
-      </c>
-      <c r="C3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>165</v>
-      </c>
-      <c r="C4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1641,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1420,15 +1649,15 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
         <v>161</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1466,15 +1695,15 @@
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -1482,7 +1711,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>49</v>
@@ -1490,7 +1719,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>48</v>
@@ -1498,7 +1727,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>47</v>
@@ -1506,7 +1735,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>46</v>
@@ -1514,7 +1743,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
@@ -1522,7 +1751,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -1530,7 +1759,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
@@ -1538,7 +1767,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>42</v>
@@ -1546,7 +1775,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>41</v>
@@ -1554,7 +1783,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>40</v>
@@ -1562,7 +1791,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>39</v>
@@ -1570,7 +1799,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -1578,7 +1807,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>37</v>
@@ -1586,7 +1815,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -1594,7 +1823,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1602,7 +1831,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1610,7 +1839,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1618,7 +1847,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -1626,7 +1855,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -1634,7 +1863,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1642,7 +1871,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
@@ -1650,7 +1879,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -1658,7 +1887,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -1666,7 +1895,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
@@ -1674,7 +1903,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
@@ -1682,7 +1911,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
         <v>24</v>
@@ -1690,7 +1919,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1698,7 +1927,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
@@ -1706,7 +1935,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -1747,10 +1976,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1760,6 +1989,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D1DBDD-2581-4D8C-8B5D-1ABD29610966}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1786,18 +2016,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1838,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1846,7 +2076,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1854,7 +2084,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1881,7 +2111,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -1892,7 +2122,7 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -1900,10 +2130,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
         <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -1911,28 +2141,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
         <v>108</v>
-      </c>
-      <c r="C11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
         <v>114</v>
-      </c>
-      <c r="C12" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>50</v>
@@ -1940,7 +2170,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>49</v>
@@ -1948,7 +2178,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>48</v>
@@ -1956,7 +2186,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>47</v>
@@ -1964,7 +2194,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>46</v>
@@ -1972,7 +2202,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>45</v>
@@ -1980,7 +2210,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>44</v>
@@ -1988,7 +2218,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>43</v>
@@ -1996,7 +2226,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>42</v>
@@ -2004,7 +2234,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>41</v>
@@ -2012,7 +2242,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>40</v>
@@ -2020,7 +2250,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>39</v>
@@ -2028,7 +2258,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>38</v>
@@ -2036,7 +2266,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>37</v>
@@ -2044,7 +2274,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>34</v>
@@ -2052,7 +2282,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>33</v>
@@ -2060,7 +2290,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>32</v>
@@ -2068,7 +2298,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>31</v>
@@ -2076,7 +2306,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>30</v>
@@ -2090,18 +2320,18 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71A6DB-F956-47B0-AA2F-995ED03DF664}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.15234375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -2111,13 +2341,312 @@
       <c r="B1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>233</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>240</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>246</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2157,7 +2686,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2197,15 +2726,15 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[draft] Adding exiftool + GTN "new version check" -- untested.
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="g:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5DB26-E407-4BF4-B218-8CB611EE990B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A95FBF-9641-41CB-ACE0-4ED94EEA1929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" activeTab="6" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="260">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -808,6 +808,35 @@
   </si>
   <si>
     <t xml:space="preserve">Error while performing  wbv_MapArea_WebMessageReceived (Please file an issue on github): </t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningExifToolVerAPIResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExifToolVerAPIResponse API Returned the following response: </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_InfoNewExifToolVersionExists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a new exifTool version available for download. 
+If you click Yes, your default browser will open to exiftool.org where you can download manually. If you click No, this message will close (but will show again next time.)
+If you download, extract the zip file, rename exiftool(-k).exe to exiftool.exe and replace the current file in your GeoTagNinja installation folder (most likely Program Files.)
+New version: </t>
+  </si>
+  <si>
+    <t>mbx_Helper_WarningGTNVerAPIResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub API Returned the following response: </t>
+  </si>
+  <si>
+    <t>mbx_frm_mainApp_InfoNewGTNVersionExists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a new GeoTagNinja version available for download. 
+If you click Yes, your default browser will open directly to the release's installer link on GitHub, which you can then install manually. If you click No, this message will close (but will show again next time.)
+New version: </t>
   </si>
 </sst>
 </file>
@@ -2320,11 +2349,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71A6DB-F956-47B0-AA2F-995ED03DF664}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2647,6 +2676,38 @@
       </c>
       <c r="C39" s="6" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>252</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="116.6" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>254</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding (better) commentary to code ++ Prepwork for time-shift capabilities. ++ Bugfixes
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A95FBF-9641-41CB-ACE0-4ED94EEA1929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922DC62-E45E-4DA8-9168-2DA74C9A7197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" activeTab="6" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" activeTab="2" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="266">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -837,6 +837,24 @@
     <t xml:space="preserve">There is a new GeoTagNinja version available for download. 
 If you click Yes, your default browser will open directly to the release's installer link on GitHub, which you can then install manually. If you click No, this message will close (but will show again next time.)
 New version: </t>
+  </si>
+  <si>
+    <t>clh_ModifyDate</t>
+  </si>
+  <si>
+    <t>clh_CreateDate</t>
+  </si>
+  <si>
+    <t>clh_OffsetTime</t>
+  </si>
+  <si>
+    <t>Modify Date</t>
+  </si>
+  <si>
+    <t>Create Date</t>
+  </si>
+  <si>
+    <t>Time Offset</t>
   </si>
 </sst>
 </file>
@@ -1697,11 +1715,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12E35C1-6424-48E0-8B92-C8A8C178A410}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1968,6 +1986,30 @@
       </c>
       <c r="C32" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>260</v>
+      </c>
+      <c r="C33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C34" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C35" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2351,7 +2393,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>

</xml_diff>

<commit_message>
Bugfixes - Fixed an issue where multiple values would be queued up for one file incorrectly (e.g. typing "50" in a value field would queue up both "5" and "50". - ...negative numbers weren't accepted in the type-in fields - ... numbers weren't saved properly when typed-in - Updated code as per issue reports 1 & 2 - Added check for exifTool version change tracking - Added check for GeoTagNinja version change tracking - Added (better) commentary to the code - Changed Settings/Edit Forms' behaviour not to block other windows.
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25615"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922DC62-E45E-4DA8-9168-2DA74C9A7197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6734CE6F-77A3-4FA9-8EC9-FC91E4DCE766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="723" activeTab="2" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13474" tabRatio="723" activeTab="4" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
     <sheet name="CheckBox" sheetId="4" r:id="rId2"/>
     <sheet name="ColumnHeader" sheetId="6" r:id="rId3"/>
     <sheet name="FileBrowser" sheetId="11" r:id="rId4"/>
-    <sheet name="GroupBox" sheetId="13" r:id="rId5"/>
-    <sheet name="Label" sheetId="3" r:id="rId6"/>
-    <sheet name="messageBox" sheetId="2" r:id="rId7"/>
-    <sheet name="PictureBox" sheetId="9" r:id="rId8"/>
-    <sheet name="RichTextBox" sheetId="5" r:id="rId9"/>
-    <sheet name="TabControl" sheetId="12" r:id="rId10"/>
-    <sheet name="TabPage" sheetId="8" r:id="rId11"/>
-    <sheet name="ToolStrip" sheetId="10" r:id="rId12"/>
-    <sheet name="ToolStripMenuItem" sheetId="14" r:id="rId13"/>
+    <sheet name="Form" sheetId="16" r:id="rId5"/>
+    <sheet name="GroupBox" sheetId="13" r:id="rId6"/>
+    <sheet name="Label" sheetId="3" r:id="rId7"/>
+    <sheet name="messageBox" sheetId="2" r:id="rId8"/>
+    <sheet name="PictureBox" sheetId="9" r:id="rId9"/>
+    <sheet name="RichTextBox" sheetId="5" r:id="rId10"/>
+    <sheet name="TabControl" sheetId="12" r:id="rId11"/>
+    <sheet name="TabPage" sheetId="8" r:id="rId12"/>
+    <sheet name="ToolStrip" sheetId="10" r:id="rId13"/>
+    <sheet name="ToolStripMenuItem" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="268">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -855,6 +856,12 @@
   </si>
   <si>
     <t>Time Offset</t>
+  </si>
+  <si>
+    <t>frm_Settings</t>
+  </si>
+  <si>
+    <t>frm_editFiledata</t>
   </si>
 </sst>
 </file>
@@ -1381,6 +1388,54 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FBCB81-7530-4E24-8050-0BE2A14003FC}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474FB6B0-1C4C-4EF7-88E9-FF86336714E7}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:C2"/>
@@ -1421,7 +1476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608740D4-3281-43A8-9891-68180F0D32F1}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C6"/>
@@ -1493,7 +1548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3CA633-2131-4005-BBF5-FD4C3AB97D80}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C3"/>
@@ -1542,7 +1597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9929B90B-AD05-4D51-B814-E736A13F0538}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:C11"/>
@@ -1717,7 +1772,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
@@ -2024,7 +2079,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2059,6 +2114,54 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F7050C-96BB-4819-95C7-C8166110F99A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D1DBDD-2581-4D8C-8B5D-1ABD29610966}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C3"/>
@@ -2106,7 +2209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF047657-9098-41C9-A35C-1E73DCC7355E}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C31"/>
@@ -2388,7 +2491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71A6DB-F956-47B0-AA2F-995ED03DF664}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C43"/>
@@ -2757,7 +2860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B470A451-D858-45D6-889B-8EF1082E77B2}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C2"/>
@@ -2795,52 +2898,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FBCB81-7530-4E24-8050-0BE2A14003FC}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="20.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Setting for Map-Reset to 0/0
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6734CE6F-77A3-4FA9-8EC9-FC91E4DCE766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B66A96E-5999-4293-AA5D-8FB19D396CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13474" tabRatio="723" activeTab="4" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13474" tabRatio="723" activeTab="6" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="270">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -862,6 +861,12 @@
   </si>
   <si>
     <t>frm_editFiledata</t>
+  </si>
+  <si>
+    <t>lbl_ResetMapToZero</t>
+  </si>
+  <si>
+    <t>Set Map to 0/0 if no GeoData</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F7050C-96BB-4819-95C7-C8166110F99A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -2212,11 +2217,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF047657-9098-41C9-A35C-1E73DCC7355E}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2484,6 +2489,14 @@
       </c>
       <c r="C31" s="5" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a "don't ask again" button
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B66A96E-5999-4293-AA5D-8FB19D396CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08A70B0-4673-4C7F-BEF1-21B09F1B3519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13474" tabRatio="723" activeTab="6" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="7" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -692,10 +692,6 @@
 Data will be discarded if you click No</t>
   </si>
   <si>
-    <t>Do you want to also assign Altitude &amp; Toponomy values?
-If you pick No, your lat/long data may become out of sync with any embedded toponomy data.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error in frm_mainApp.NavigateMapGo (string HTMLCode) (Please file an issue on github): </t>
   </si>
   <si>
@@ -863,10 +859,15 @@
     <t>frm_editFiledata</t>
   </si>
   <si>
-    <t>lbl_ResetMapToZero</t>
-  </si>
-  <si>
     <t>Set Map to 0/0 if no GeoData</t>
+  </si>
+  <si>
+    <t>ckb_ResetMapToZero</t>
+  </si>
+  <si>
+    <t>Do you want to also assign Altitude &amp; Toponomy values?
+If you pick No, your lat/long data may become out of sync with any embedded toponomy data.
+If you click 'stop asking' it will take the answer as Yes and won't ask again this session. Restart to reset.</t>
   </si>
 </sst>
 </file>
@@ -1272,14 +1273,14 @@
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" customWidth="1"/>
-    <col min="3" max="3" width="41.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1330,7 +1331,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>166</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -1402,13 +1403,13 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.15234375" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1450,14 +1451,14 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.61328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.61328125" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1491,13 +1492,13 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.921875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1532,7 +1533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -1563,14 +1564,14 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1612,14 +1613,14 @@
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>162</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>150</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -1718,21 +1719,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4D1A38-DF6E-4C32-B78F-C0F0A755128B}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3828125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1759,12 +1760,20 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>160</v>
       </c>
       <c r="C4" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1782,14 +1791,14 @@
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.69140625" customWidth="1"/>
-    <col min="3" max="3" width="18.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>111</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1864,7 +1873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1880,7 +1889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -1896,7 +1905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -1904,7 +1913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1912,7 +1921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1920,7 +1929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -1960,7 +1969,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1992,7 +2001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -2016,7 +2025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2024,7 +2033,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -2032,7 +2041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2048,28 +2057,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>259</v>
+      </c>
+      <c r="C33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>260</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>261</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>262</v>
-      </c>
-      <c r="C35" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2087,14 +2096,14 @@
       <selection pane="bottomLeft" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.61328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.61328125" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -2127,14 +2136,14 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2145,17 +2154,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
         <v>116</v>
@@ -2176,13 +2185,13 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3828125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2193,7 +2202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2201,7 +2210,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -2217,21 +2226,21 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF047657-9098-41C9-A35C-1E73DCC7355E}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.61328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.61328125" customWidth="1"/>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2259,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2258,7 +2267,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2266,7 +2275,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2274,7 +2283,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2293,7 +2302,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2304,7 +2313,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2323,7 +2332,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2339,7 +2348,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -2355,7 +2364,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -2363,7 +2372,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -2379,7 +2388,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -2403,7 +2412,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -2411,7 +2420,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -2419,7 +2428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -2451,7 +2460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -2459,7 +2468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -2467,7 +2476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -2475,7 +2484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2483,20 +2492,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>140</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>268</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2509,19 +2510,19 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.15234375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2532,87 +2533,87 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>184</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>190</v>
       </c>
@@ -2628,7 +2629,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>191</v>
       </c>
@@ -2636,7 +2637,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>192</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>193</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>208</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -2668,23 +2669,23 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -2692,15 +2693,15 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>186</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -2716,7 +2717,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>189</v>
       </c>
@@ -2724,148 +2725,148 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>221</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C30" s="6" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="C31" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C32" s="6" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="C33" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C33" s="6" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>242</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>242</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="C35" s="6" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>245</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="6" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+      <c r="C39" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>251</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C40" s="6" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="116.6" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+      <c r="C41" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C41" s="6" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="C42" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C42" s="6" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+      <c r="C43" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2883,13 +2884,13 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.4609375" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Changes to "do not ask again" map/loc logic.
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08A70B0-4673-4C7F-BEF1-21B09F1B3519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E4C042-198A-4EE1-BF74-F718EA66C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="7" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="1" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="276">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -716,9 +716,6 @@
     <t>mbx_frm_mainApp_QuestionDontShowIncompatibleFileWarningAgain</t>
   </si>
   <si>
-    <t>mbx_frm_mainApp_QuestionAddToponomy</t>
-  </si>
-  <si>
     <t>mbx_frm_mainApp_QuestionFileQIsNotEmpty</t>
   </si>
   <si>
@@ -865,9 +862,30 @@
     <t>ckb_ResetMapToZero</t>
   </si>
   <si>
-    <t>Do you want to also assign Altitude &amp; Toponomy values?
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Don't Ask again</t>
+  </si>
+  <si>
+    <t>btn_Yes</t>
+  </si>
+  <si>
+    <t>btn_No</t>
+  </si>
+  <si>
+    <t>Do you want to also assign Altitude and Toponomy values?
 If you pick No, your lat/long data may become out of sync with any embedded toponomy data.
 If you click 'stop asking' it will take the answer as Yes and won't ask again this session. Restart to reset.</t>
+  </si>
+  <si>
+    <t>lbl_QuestionAddToponomy</t>
+  </si>
+  <si>
+    <t>ckb_QuestionAddToponomyDontAskAgain</t>
   </si>
 </sst>
 </file>
@@ -938,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -951,6 +969,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,11 +1285,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D057A75-CE07-4B70-81C2-6848CE46E100}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,6 +1404,22 @@
       </c>
       <c r="C13" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1719,9 +1754,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4D1A38-DF6E-4C32-B78F-C0F0A755128B}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
@@ -1770,10 +1805,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2059,26 +2102,26 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2156,7 +2199,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>154</v>
@@ -2164,7 +2207,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" t="s">
         <v>116</v>
@@ -2226,11 +2269,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF047657-9098-41C9-A35C-1E73DCC7355E}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="A32:C32"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2500,6 +2543,15 @@
         <v>30</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2508,11 +2560,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71A6DB-F956-47B0-AA2F-995ED03DF664}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,7 +2587,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>179</v>
@@ -2543,7 +2595,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>181</v>
@@ -2551,7 +2603,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>194</v>
@@ -2559,7 +2611,7 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>180</v>
@@ -2567,7 +2619,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>182</v>
@@ -2575,7 +2627,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>198</v>
@@ -2583,7 +2635,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>197</v>
@@ -2591,7 +2643,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>196</v>
@@ -2599,7 +2651,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>195</v>
@@ -2607,7 +2659,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>183</v>
@@ -2682,7 +2734,7 @@
         <v>212</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2727,66 +2779,66 @@
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -2794,79 +2846,71 @@
         <v>241</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>195</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>244</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>245</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>213</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
         <v>257</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to ExifTool "newest" version querying.
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25813"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E4C042-198A-4EE1-BF74-F718EA66C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B45410-4550-4A56-B774-2DFD4283087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="1" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="7" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Button" sheetId="1" r:id="rId1"/>
@@ -812,12 +812,6 @@
     <t>mbx_frm_mainApp_InfoNewExifToolVersionExists</t>
   </si>
   <si>
-    <t xml:space="preserve">There is a new exifTool version available for download. 
-If you click Yes, your default browser will open to exiftool.org where you can download manually. If you click No, this message will close (but will show again next time.)
-If you download, extract the zip file, rename exiftool(-k).exe to exiftool.exe and replace the current file in your GeoTagNinja installation folder (most likely Program Files.)
-New version: </t>
-  </si>
-  <si>
     <t>mbx_Helper_WarningGTNVerAPIResponse</t>
   </si>
   <si>
@@ -886,6 +880,12 @@
   </si>
   <si>
     <t>ckb_QuestionAddToponomyDontAskAgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a new exifTool version available for download. 
+If you click Yes, your default browser will open to exiftool.org where you can download manually. If you click No, this message will close (and you won't be notified again until yet another new version is out.)
+If you download, extract the zip file, rename exiftool(-k).exe to exiftool.exe and replace the current file in your GeoTagNinja installation folder's Resources subfolder (most likely Program Files\GeoTagNinja\Resources.)
+New version: </t>
   </si>
 </sst>
 </file>
@@ -956,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -969,7 +969,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,18 +1407,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1756,7 +1755,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
@@ -1805,18 +1804,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2102,26 +2101,26 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2199,7 +2198,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
         <v>154</v>
@@ -2207,7 +2206,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
         <v>116</v>
@@ -2269,11 +2268,11 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF047657-9098-41C9-A35C-1E73DCC7355E}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2544,13 +2543,15 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8" t="s">
+      <c r="A32" t="s">
         <v>273</v>
       </c>
+      <c r="C32" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2562,9 +2563,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2894,23 +2895,23 @@
         <v>252</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>253</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>255</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2925,7 +2926,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Multi-Select capability to the map. + Partial French Translations
</commit_message>
<xml_diff>
--- a/extraFiles/english.xlsx
+++ b/extraFiles/english.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25822"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Sajat\Jobs\Nem_Aktualis\Apps\GeoTagNinja\extraFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B45410-4550-4A56-B774-2DFD4283087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC7361B-DF47-43A6-AC53-E2F893EE3AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" tabRatio="723" activeTab="7" xr2:uid="{D4CAFA08-10F0-418D-A9E0-593D628FE0B2}"/>
   </bookViews>
@@ -21,12 +21,13 @@
     <sheet name="GroupBox" sheetId="13" r:id="rId6"/>
     <sheet name="Label" sheetId="3" r:id="rId7"/>
     <sheet name="messageBox" sheetId="2" r:id="rId8"/>
-    <sheet name="PictureBox" sheetId="9" r:id="rId9"/>
-    <sheet name="RichTextBox" sheetId="5" r:id="rId10"/>
-    <sheet name="TabControl" sheetId="12" r:id="rId11"/>
-    <sheet name="TabPage" sheetId="8" r:id="rId12"/>
-    <sheet name="ToolStrip" sheetId="10" r:id="rId13"/>
-    <sheet name="ToolStripMenuItem" sheetId="14" r:id="rId14"/>
+    <sheet name="MenuStrip" sheetId="17" r:id="rId9"/>
+    <sheet name="PictureBox" sheetId="9" r:id="rId10"/>
+    <sheet name="RichTextBox" sheetId="5" r:id="rId11"/>
+    <sheet name="TabControl" sheetId="12" r:id="rId12"/>
+    <sheet name="TabPage" sheetId="8" r:id="rId13"/>
+    <sheet name="ToolStrip" sheetId="10" r:id="rId14"/>
+    <sheet name="ToolStripMenuItem" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="281">
   <si>
     <t>tpg_Map</t>
   </si>
@@ -886,6 +887,21 @@
 If you click Yes, your default browser will open to exiftool.org where you can download manually. If you click No, this message will close (and you won't be notified again until yet another new version is out.)
 If you download, extract the zip file, rename exiftool(-k).exe to exiftool.exe and replace the current file in your GeoTagNinja installation folder's Resources subfolder (most likely Program Files\GeoTagNinja\Resources.)
 New version: </t>
+  </si>
+  <si>
+    <t>mns_File</t>
+  </si>
+  <si>
+    <t>mns_Settings</t>
+  </si>
+  <si>
+    <t>mns_Help</t>
+  </si>
+  <si>
+    <t>mbx_frm_Settings_cbx_Language_TextChanged</t>
+  </si>
+  <si>
+    <t>Please restart the app for the language change to take place.</t>
   </si>
 </sst>
 </file>
@@ -1428,6 +1444,46 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B470A451-D858-45D6-889B-8EF1082E77B2}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FBCB81-7530-4E24-8050-0BE2A14003FC}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C3"/>
@@ -1475,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474FB6B0-1C4C-4EF7-88E9-FF86336714E7}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:C2"/>
@@ -1516,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608740D4-3281-43A8-9891-68180F0D32F1}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C6"/>
@@ -1588,14 +1644,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3CA633-2131-4005-BBF5-FD4C3AB97D80}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1637,7 +1693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9929B90B-AD05-4D51-B814-E736A13F0538}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:C11"/>
@@ -2561,11 +2617,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA71A6DB-F956-47B0-AA2F-995ED03DF664}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2914,25 +2970,33 @@
         <v>256</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>279</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B470A451-D858-45D6-889B-8EF1082E77B2}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415C8C92-2CBB-449A-9A72-B19209671BCB}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2948,10 +3012,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>276</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>